<commit_message>
excell export, refs directory
</commit_message>
<xml_diff>
--- a/src/monitoring_data.xlsx
+++ b/src/monitoring_data.xlsx
@@ -14,9 +14,29 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="6">
   <si>
-    <t>Monitoring Data</t>
+    <t>Time</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Flow, kg/s</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>DeltaP, Pa</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>P, Pa</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Temp, K</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Temp2, K</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -321,18 +341,1273 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:T21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="8.38" customWidth="1"/>
+    <col min="1" max="20" width="8.38" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20">
+      <c r="A2">
+        <v>1741972681</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>-26406.918237599995</v>
+      </c>
+      <c r="D2">
+        <v>92461.84491360001</v>
+      </c>
+      <c r="E2">
+        <v>297.51</v>
+      </c>
+      <c r="F2">
+        <v>299.56</v>
+      </c>
+      <c r="G2">
+        <v>72053.3650224</v>
+      </c>
+      <c r="H2">
+        <v>208500.60051120003</v>
+      </c>
+      <c r="I2">
+        <v>112663.48210319999</v>
+      </c>
+      <c r="J2">
+        <v>248076.504084</v>
+      </c>
+      <c r="K2">
+        <v>85015.507656</v>
+      </c>
+      <c r="L2">
+        <v>209259.0237504</v>
+      </c>
+      <c r="M2">
+        <v>73914.9493368</v>
+      </c>
+      <c r="N2">
+        <v>172096.2850296</v>
+      </c>
+      <c r="O2">
+        <v>1.5932451846147049</v>
+      </c>
+      <c r="P2">
+        <v>1.9211093235729242</v>
+      </c>
+      <c r="Q2">
+        <v>1.6195926527992623</v>
+      </c>
+      <c r="R2">
+        <v>1.3336656169424448</v>
+      </c>
+      <c r="S2">
+        <v>646.7612777929336</v>
+      </c>
+      <c r="T2">
+        <v>36.33140862329453</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20">
+      <c r="A3">
+        <v>1741972682</v>
+      </c>
+      <c r="B3">
+        <v>0.809789441442755</v>
+      </c>
+      <c r="C3">
+        <v>4481.591867999989</v>
+      </c>
+      <c r="D3">
+        <v>91841.3168088</v>
+      </c>
+      <c r="E3">
+        <v>302.85999999999996</v>
+      </c>
+      <c r="F3">
+        <v>300.39</v>
+      </c>
+      <c r="G3">
+        <v>130658.79714240001</v>
+      </c>
+      <c r="H3">
+        <v>233597.51497200003</v>
+      </c>
+      <c r="I3">
+        <v>130107.2166048</v>
+      </c>
+      <c r="J3">
+        <v>257729.16349200002</v>
+      </c>
+      <c r="K3">
+        <v>126590.8906776</v>
+      </c>
+      <c r="L3">
+        <v>230012.2414776</v>
+      </c>
+      <c r="M3">
+        <v>121281.9280032</v>
+      </c>
+      <c r="N3">
+        <v>255522.8413416</v>
+      </c>
+      <c r="O3">
+        <v>1.7590054195874076</v>
+      </c>
+      <c r="P3">
+        <v>1.977187853115395</v>
+      </c>
+      <c r="Q3">
+        <v>1.7386002983993725</v>
+      </c>
+      <c r="R3">
+        <v>1.9717302331031612</v>
+      </c>
+      <c r="S3">
+        <v>919.5629657677797</v>
+      </c>
+      <c r="T3">
+        <v>12.816050065201326</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20">
+      <c r="A4">
+        <v>1741972683</v>
+      </c>
+      <c r="B4">
+        <v>2.6013627227135028</v>
+      </c>
+      <c r="C4">
+        <v>56468.0575368</v>
+      </c>
+      <c r="D4">
+        <v>129900.3739032</v>
+      </c>
+      <c r="E4">
+        <v>296.78</v>
+      </c>
+      <c r="F4">
+        <v>296.04999999999995</v>
+      </c>
+      <c r="G4">
+        <v>90876.050868</v>
+      </c>
+      <c r="H4">
+        <v>168511.0115352</v>
+      </c>
+      <c r="I4">
+        <v>80258.1255192</v>
+      </c>
+      <c r="J4">
+        <v>150929.3818992</v>
+      </c>
+      <c r="K4">
+        <v>101907.66162</v>
+      </c>
+      <c r="L4">
+        <v>223531.17016080001</v>
+      </c>
+      <c r="M4">
+        <v>132451.4338896</v>
+      </c>
+      <c r="N4">
+        <v>224289.5934</v>
+      </c>
+      <c r="O4">
+        <v>1.288541551877632</v>
+      </c>
+      <c r="P4">
+        <v>1.15717487748923</v>
+      </c>
+      <c r="Q4">
+        <v>1.7410343736230252</v>
+      </c>
+      <c r="R4">
+        <v>1.674913207280861</v>
+      </c>
+      <c r="S4">
+        <v>225.3305146218286</v>
+      </c>
+      <c r="T4">
+        <v>39.84257679121576</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20">
+      <c r="A5">
+        <v>1741972684</v>
+      </c>
+      <c r="B5">
+        <v>2.3011754155793462</v>
+      </c>
+      <c r="C5">
+        <v>38748.53276640001</v>
+      </c>
+      <c r="D5">
+        <v>120937.19016720001</v>
+      </c>
+      <c r="E5">
+        <v>297.34999999999997</v>
+      </c>
+      <c r="F5">
+        <v>301.2</v>
+      </c>
+      <c r="G5">
+        <v>76259.1666216</v>
+      </c>
+      <c r="H5">
+        <v>212499.55940880004</v>
+      </c>
+      <c r="I5">
+        <v>105010.302144</v>
+      </c>
+      <c r="J5">
+        <v>220566.42477120002</v>
+      </c>
+      <c r="K5">
+        <v>92668.6876152</v>
+      </c>
+      <c r="L5">
+        <v>203053.74270240002</v>
+      </c>
+      <c r="M5">
+        <v>82188.6574008</v>
+      </c>
+      <c r="N5">
+        <v>206018.488092</v>
+      </c>
+      <c r="O5">
+        <v>1.6259081290945516</v>
+      </c>
+      <c r="P5">
+        <v>1.6993452408145833</v>
+      </c>
+      <c r="Q5">
+        <v>1.567902782705729</v>
+      </c>
+      <c r="R5">
+        <v>1.5888880910669267</v>
+      </c>
+      <c r="S5">
+        <v>281.6840558871461</v>
+      </c>
+      <c r="T5">
+        <v>8.111173152634647</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20">
+      <c r="A6">
+        <v>1741972685</v>
+      </c>
+      <c r="B6">
+        <v>2.646460932002791</v>
+      </c>
+      <c r="C6">
+        <v>46608.555427200015</v>
+      </c>
+      <c r="D6">
+        <v>137829.34413120002</v>
+      </c>
+      <c r="E6">
+        <v>299.46999999999997</v>
+      </c>
+      <c r="F6">
+        <v>299.53999999999996</v>
+      </c>
+      <c r="G6">
+        <v>75431.7958152</v>
+      </c>
+      <c r="H6">
+        <v>176302.08662880003</v>
+      </c>
+      <c r="I6">
+        <v>69364.4099016</v>
+      </c>
+      <c r="J6">
+        <v>142586.726268</v>
+      </c>
+      <c r="K6">
+        <v>112801.3772376</v>
+      </c>
+      <c r="L6">
+        <v>218773.788024</v>
+      </c>
+      <c r="M6">
+        <v>72260.20772399999</v>
+      </c>
+      <c r="N6">
+        <v>152308.33324319997</v>
+      </c>
+      <c r="O6">
+        <v>1.3662665484510854</v>
+      </c>
+      <c r="P6">
+        <v>1.0997170440384454</v>
+      </c>
+      <c r="Q6">
+        <v>1.675939968529213</v>
+      </c>
+      <c r="R6">
+        <v>1.1769812438130236</v>
+      </c>
+      <c r="S6">
+        <v>200.98179952373306</v>
+      </c>
+      <c r="T6">
+        <v>43.333952806774704</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20">
+      <c r="A7">
+        <v>1741972686</v>
+      </c>
+      <c r="B7">
+        <v>2.707664209526076</v>
+      </c>
+      <c r="C7">
+        <v>53365.4170128</v>
+      </c>
+      <c r="D7">
+        <v>136933.0257576</v>
+      </c>
+      <c r="E7">
+        <v>297.33</v>
+      </c>
+      <c r="F7">
+        <v>299.46</v>
+      </c>
+      <c r="G7">
+        <v>118386.13018080001</v>
+      </c>
+      <c r="H7">
+        <v>232218.56362800003</v>
+      </c>
+      <c r="I7">
+        <v>135829.86468240002</v>
+      </c>
+      <c r="J7">
+        <v>249110.71759200003</v>
+      </c>
+      <c r="K7">
+        <v>93771.8486904</v>
+      </c>
+      <c r="L7">
+        <v>183610.528752</v>
+      </c>
+      <c r="M7">
+        <v>121144.0328688</v>
+      </c>
+      <c r="N7">
+        <v>213533.7729168</v>
+      </c>
+      <c r="O7">
+        <v>1.7819896445511718</v>
+      </c>
+      <c r="P7">
+        <v>1.8897164960047375</v>
+      </c>
+      <c r="Q7">
+        <v>1.4086461705702784</v>
+      </c>
+      <c r="R7">
+        <v>1.6045657402887512</v>
+      </c>
+      <c r="S7">
+        <v>246.88874004007326</v>
+      </c>
+      <c r="T7">
+        <v>28.785413477589906</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20">
+      <c r="A8">
+        <v>1741972688</v>
+      </c>
+      <c r="B8">
+        <v>0.4022693008879437</v>
+      </c>
+      <c r="C8">
+        <v>827.3708063999802</v>
+      </c>
+      <c r="D8">
+        <v>117696.6545088</v>
+      </c>
+      <c r="E8">
+        <v>300.14</v>
+      </c>
+      <c r="F8">
+        <v>301.69</v>
+      </c>
+      <c r="G8">
+        <v>81981.8146992</v>
+      </c>
+      <c r="H8">
+        <v>203743.2183744</v>
+      </c>
+      <c r="I8">
+        <v>115972.9653288</v>
+      </c>
+      <c r="J8">
+        <v>186851.0644104</v>
+      </c>
+      <c r="K8">
+        <v>130107.2166048</v>
+      </c>
+      <c r="L8">
+        <v>250696.51163760002</v>
+      </c>
+      <c r="M8">
+        <v>118317.1826136</v>
+      </c>
+      <c r="N8">
+        <v>249248.6127264</v>
+      </c>
+      <c r="O8">
+        <v>1.5706939525080004</v>
+      </c>
+      <c r="P8">
+        <v>1.35649662802757</v>
+      </c>
+      <c r="Q8">
+        <v>1.911768132729978</v>
+      </c>
+      <c r="R8">
+        <v>1.9191526522384403</v>
+      </c>
+      <c r="S8">
+        <v>1679.996795824728</v>
+      </c>
+      <c r="T8">
+        <v>33.30256006628621</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20">
+      <c r="A9">
+        <v>1741972689</v>
+      </c>
+      <c r="B9">
+        <v>0.26007318202771706</v>
+      </c>
+      <c r="C9">
+        <v>482.63297040000907</v>
+      </c>
+      <c r="D9">
+        <v>84532.8746856</v>
+      </c>
+      <c r="E9">
+        <v>296.4</v>
+      </c>
+      <c r="F9">
+        <v>297.45</v>
+      </c>
+      <c r="G9">
+        <v>91772.3692416</v>
+      </c>
+      <c r="H9">
+        <v>224013.80313120002</v>
+      </c>
+      <c r="I9">
+        <v>107285.5718616</v>
+      </c>
+      <c r="J9">
+        <v>244146.4927536</v>
+      </c>
+      <c r="K9">
+        <v>134381.96577120002</v>
+      </c>
+      <c r="L9">
+        <v>215326.40966400004</v>
+      </c>
+      <c r="M9">
+        <v>83291.81847600001</v>
+      </c>
+      <c r="N9">
+        <v>153342.54675120002</v>
+      </c>
+      <c r="O9">
+        <v>1.7404622947932127</v>
+      </c>
+      <c r="P9">
+        <v>1.898655778661568</v>
+      </c>
+      <c r="Q9">
+        <v>1.5705877823092909</v>
+      </c>
+      <c r="R9">
+        <v>1.1680931109439254</v>
+      </c>
+      <c r="S9">
+        <v>2452.3093526914627</v>
+      </c>
+      <c r="T9">
+        <v>45.819109164849344</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20">
+      <c r="A10">
+        <v>1741972690</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>-14272.14641039999</v>
+      </c>
+      <c r="D10">
+        <v>85911.82602960001</v>
+      </c>
+      <c r="E10">
+        <v>302.96</v>
+      </c>
+      <c r="F10">
+        <v>294.34999999999997</v>
+      </c>
+      <c r="G10">
+        <v>133554.5949648</v>
+      </c>
+      <c r="H10">
+        <v>261314.4369864</v>
+      </c>
+      <c r="I10">
+        <v>102252.39945600001</v>
+      </c>
+      <c r="J10">
+        <v>234218.04307680004</v>
+      </c>
+      <c r="K10">
+        <v>129073.00309680002</v>
+      </c>
+      <c r="L10">
+        <v>252764.93865360005</v>
+      </c>
+      <c r="M10">
+        <v>133830.3852336</v>
+      </c>
+      <c r="N10">
+        <v>262279.7029272</v>
+      </c>
+      <c r="O10">
+        <v>2.0219085820960307</v>
+      </c>
+      <c r="P10">
+        <v>1.8310936630144394</v>
+      </c>
+      <c r="Q10">
+        <v>1.9559880510317982</v>
+      </c>
+      <c r="R10">
+        <v>2.0298243263295794</v>
+      </c>
+      <c r="S10">
+        <v>783.8814622471848</v>
+      </c>
+      <c r="T10">
+        <v>10.140852814425832</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20">
+      <c r="A11">
+        <v>1741972691</v>
+      </c>
+      <c r="B11">
+        <v>0.2568514408351907</v>
+      </c>
+      <c r="C11">
+        <v>482.63297039997997</v>
+      </c>
+      <c r="D11">
+        <v>83774.4514464</v>
+      </c>
+      <c r="E11">
+        <v>301.19</v>
+      </c>
+      <c r="F11">
+        <v>296.02</v>
+      </c>
+      <c r="G11">
+        <v>111905.058864</v>
+      </c>
+      <c r="H11">
+        <v>191539.49898000003</v>
+      </c>
+      <c r="I11">
+        <v>129417.74093279999</v>
+      </c>
+      <c r="J11">
+        <v>212844.2972448</v>
+      </c>
+      <c r="K11">
+        <v>122454.0366456</v>
+      </c>
+      <c r="L11">
+        <v>240147.533856</v>
+      </c>
+      <c r="M11">
+        <v>104045.03620320001</v>
+      </c>
+      <c r="N11">
+        <v>218980.63072560003</v>
+      </c>
+      <c r="O11">
+        <v>1.4353700573466364</v>
+      </c>
+      <c r="P11">
+        <v>1.5730016450335857</v>
+      </c>
+      <c r="Q11">
+        <v>1.8534593041589964</v>
+      </c>
+      <c r="R11">
+        <v>1.7020616844314516</v>
+      </c>
+      <c r="S11">
+        <v>2555.5210707120023</v>
+      </c>
+      <c r="T11">
+        <v>25.47812808624895</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20">
+      <c r="A12">
+        <v>1741972692</v>
+      </c>
+      <c r="B12">
+        <v>2.6539058333361734</v>
+      </c>
+      <c r="C12">
+        <v>46263.817591200015</v>
+      </c>
+      <c r="D12">
+        <v>137691.44899680003</v>
+      </c>
+      <c r="E12">
+        <v>296.29999999999995</v>
+      </c>
+      <c r="F12">
+        <v>300.92999999999995</v>
+      </c>
+      <c r="G12">
+        <v>111698.21616240001</v>
+      </c>
+      <c r="H12">
+        <v>236424.36522720003</v>
+      </c>
+      <c r="I12">
+        <v>119489.29125600001</v>
+      </c>
+      <c r="J12">
+        <v>208500.60051120003</v>
+      </c>
+      <c r="K12">
+        <v>83636.556312</v>
+      </c>
+      <c r="L12">
+        <v>194159.5065336</v>
+      </c>
+      <c r="M12">
+        <v>73777.0542024</v>
+      </c>
+      <c r="N12">
+        <v>196779.5140872</v>
+      </c>
+      <c r="O12">
+        <v>1.8232713696112575</v>
+      </c>
+      <c r="P12">
+        <v>1.5585860807062293</v>
+      </c>
+      <c r="Q12">
+        <v>1.5012385781459003</v>
+      </c>
+      <c r="R12">
+        <v>1.5122194703104306</v>
+      </c>
+      <c r="S12">
+        <v>240.97748376906014</v>
+      </c>
+      <c r="T12">
+        <v>20.14179231827427</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20">
+      <c r="A13">
+        <v>1741972693</v>
+      </c>
+      <c r="B13">
+        <v>2.2869915237286373</v>
+      </c>
+      <c r="C13">
+        <v>42954.33436559999</v>
+      </c>
+      <c r="D13">
+        <v>116110.86046319999</v>
+      </c>
+      <c r="E13">
+        <v>294.51</v>
+      </c>
+      <c r="F13">
+        <v>294.75</v>
+      </c>
+      <c r="G13">
+        <v>130176.16417200002</v>
+      </c>
+      <c r="H13">
+        <v>199744.25947680004</v>
+      </c>
+      <c r="I13">
+        <v>111215.58319200002</v>
+      </c>
+      <c r="J13">
+        <v>248765.97975600002</v>
+      </c>
+      <c r="K13">
+        <v>74880.2152776</v>
+      </c>
+      <c r="L13">
+        <v>147550.9511064</v>
+      </c>
+      <c r="M13">
+        <v>127625.10418560001</v>
+      </c>
+      <c r="N13">
+        <v>240078.5862888</v>
+      </c>
+      <c r="O13">
+        <v>1.432884755850862</v>
+      </c>
+      <c r="P13">
+        <v>1.9429181536016813</v>
+      </c>
+      <c r="Q13">
+        <v>1.1419654098258059</v>
+      </c>
+      <c r="R13">
+        <v>1.8448377466954398</v>
+      </c>
+      <c r="S13">
+        <v>278.20855477419525</v>
+      </c>
+      <c r="T13">
+        <v>50.35375350733996</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20">
+      <c r="A14">
+        <v>1741972694</v>
+      </c>
+      <c r="B14">
+        <v>1.557549234531337</v>
+      </c>
+      <c r="C14">
+        <v>12272.66696159997</v>
+      </c>
+      <c r="D14">
+        <v>128797.21282799999</v>
+      </c>
+      <c r="E14">
+        <v>299.29999999999995</v>
+      </c>
+      <c r="F14">
+        <v>300.51</v>
+      </c>
+      <c r="G14">
+        <v>113284.01020799999</v>
+      </c>
+      <c r="H14">
+        <v>248559.1370544</v>
+      </c>
+      <c r="I14">
+        <v>126039.31014</v>
+      </c>
+      <c r="J14">
+        <v>219463.263696</v>
+      </c>
+      <c r="K14">
+        <v>78603.38390639999</v>
+      </c>
+      <c r="L14">
+        <v>205260.0648528</v>
+      </c>
+      <c r="M14">
+        <v>98873.96866320001</v>
+      </c>
+      <c r="N14">
+        <v>235459.0992864</v>
+      </c>
+      <c r="O14">
+        <v>1.9215718264540562</v>
+      </c>
+      <c r="P14">
+        <v>1.640690652000439</v>
+      </c>
+      <c r="Q14">
+        <v>1.5809962386198093</v>
+      </c>
+      <c r="R14">
+        <v>1.8212753193206022</v>
+      </c>
+      <c r="S14">
+        <v>447.1469589525058</v>
+      </c>
+      <c r="T14">
+        <v>19.560567070502312</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20">
+      <c r="A15">
+        <v>1741972695</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>-38334.84736319998</v>
+      </c>
+      <c r="D15">
+        <v>93427.1108544</v>
+      </c>
+      <c r="E15">
+        <v>297.02</v>
+      </c>
+      <c r="F15">
+        <v>299.03999999999996</v>
+      </c>
+      <c r="G15">
+        <v>98184.49299120001</v>
+      </c>
+      <c r="H15">
+        <v>209259.0237504</v>
+      </c>
+      <c r="I15">
+        <v>95357.64273600001</v>
+      </c>
+      <c r="J15">
+        <v>186713.169276</v>
+      </c>
+      <c r="K15">
+        <v>93565.0059888</v>
+      </c>
+      <c r="L15">
+        <v>217532.7318144</v>
+      </c>
+      <c r="M15">
+        <v>70812.30881280001</v>
+      </c>
+      <c r="N15">
+        <v>204294.798912</v>
+      </c>
+      <c r="O15">
+        <v>1.619543413646154</v>
+      </c>
+      <c r="P15">
+        <v>1.4334524413814993</v>
+      </c>
+      <c r="Q15">
+        <v>1.6872553175223082</v>
+      </c>
+      <c r="R15">
+        <v>1.562996632228709</v>
+      </c>
+      <c r="S15">
+        <v>630.3247804778671</v>
+      </c>
+      <c r="T15">
+        <v>16.106165202541693</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20">
+      <c r="A16">
+        <v>1741972696</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>-3792.1161960000027</v>
+      </c>
+      <c r="D16">
+        <v>108664.52320560001</v>
+      </c>
+      <c r="E16">
+        <v>294.73999999999995</v>
+      </c>
+      <c r="F16">
+        <v>298.98999999999995</v>
+      </c>
+      <c r="G16">
+        <v>92875.5303168</v>
+      </c>
+      <c r="H16">
+        <v>172372.0752984</v>
+      </c>
+      <c r="I16">
+        <v>81568.12929600001</v>
+      </c>
+      <c r="J16">
+        <v>162443.62562160002</v>
+      </c>
+      <c r="K16">
+        <v>115490.3323584</v>
+      </c>
+      <c r="L16">
+        <v>236906.9981976</v>
+      </c>
+      <c r="M16">
+        <v>113490.8529096</v>
+      </c>
+      <c r="N16">
+        <v>198434.2557</v>
+      </c>
+      <c r="O16">
+        <v>1.311799737186064</v>
+      </c>
+      <c r="P16">
+        <v>1.2499207169496094</v>
+      </c>
+      <c r="Q16">
+        <v>1.8285100999227988</v>
+      </c>
+      <c r="R16">
+        <v>1.488986736635078</v>
+      </c>
+      <c r="S16">
+        <v>587.921729069355</v>
+      </c>
+      <c r="T16">
+        <v>39.365062005043555</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20">
+      <c r="A17">
+        <v>1741972697</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <v>-35990.630078400005</v>
+      </c>
+      <c r="D17">
+        <v>72673.8931272</v>
+      </c>
+      <c r="E17">
+        <v>295.96</v>
+      </c>
+      <c r="F17">
+        <v>299.46</v>
+      </c>
+      <c r="G17">
+        <v>81499.1817288</v>
+      </c>
+      <c r="H17">
+        <v>216981.1512768</v>
+      </c>
+      <c r="I17">
+        <v>122867.7220488</v>
+      </c>
+      <c r="J17">
+        <v>210224.2896912</v>
+      </c>
+      <c r="K17">
+        <v>82533.3952368</v>
+      </c>
+      <c r="L17">
+        <v>195193.7200416</v>
+      </c>
+      <c r="M17">
+        <v>71984.4174552</v>
+      </c>
+      <c r="N17">
+        <v>191056.8660096</v>
+      </c>
+      <c r="O17">
+        <v>1.6717948175833253</v>
+      </c>
+      <c r="P17">
+        <v>1.5661316911939371</v>
+      </c>
+      <c r="Q17">
+        <v>1.512654123452704</v>
+      </c>
+      <c r="R17">
+        <v>1.4724101846716164</v>
+      </c>
+      <c r="S17">
+        <v>622.2990816901583</v>
+      </c>
+      <c r="T17">
+        <v>12.81600045882646</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20">
+      <c r="A18">
+        <v>1741972698</v>
+      </c>
+      <c r="B18">
+        <v>2.10941970396002</v>
+      </c>
+      <c r="C18">
+        <v>30612.71983680001</v>
+      </c>
+      <c r="D18">
+        <v>116869.28370240002</v>
+      </c>
+      <c r="E18">
+        <v>295.83</v>
+      </c>
+      <c r="F18">
+        <v>297</v>
+      </c>
+      <c r="G18">
+        <v>107699.2572648</v>
+      </c>
+      <c r="H18">
+        <v>239182.26791520003</v>
+      </c>
+      <c r="I18">
+        <v>130245.1117392</v>
+      </c>
+      <c r="J18">
+        <v>242560.698708</v>
+      </c>
+      <c r="K18">
+        <v>74328.63474000001</v>
+      </c>
+      <c r="L18">
+        <v>162236.78292000003</v>
+      </c>
+      <c r="M18">
+        <v>73570.21150080001</v>
+      </c>
+      <c r="N18">
+        <v>195469.51031040002</v>
+      </c>
+      <c r="O18">
+        <v>1.8606635355051766</v>
+      </c>
+      <c r="P18">
+        <v>1.8533682740325081</v>
+      </c>
+      <c r="Q18">
+        <v>1.261372878237543</v>
+      </c>
+      <c r="R18">
+        <v>1.5125201143929012</v>
+      </c>
+      <c r="S18">
+        <v>307.5691760150115</v>
+      </c>
+      <c r="T18">
+        <v>36.94806432203796</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20">
+      <c r="A19">
+        <v>1741972699</v>
+      </c>
+      <c r="B19">
+        <v>2.6087253295479362</v>
+      </c>
+      <c r="C19">
+        <v>47435.926233599996</v>
+      </c>
+      <c r="D19">
+        <v>135485.1268464</v>
+      </c>
+      <c r="E19">
+        <v>302.2</v>
+      </c>
+      <c r="F19">
+        <v>299.71999999999997</v>
+      </c>
+      <c r="G19">
+        <v>80602.86335520001</v>
+      </c>
+      <c r="H19">
+        <v>149757.27325680002</v>
+      </c>
+      <c r="I19">
+        <v>88324.9908816</v>
+      </c>
+      <c r="J19">
+        <v>203329.5329712</v>
+      </c>
+      <c r="K19">
+        <v>71570.732052</v>
+      </c>
+      <c r="L19">
+        <v>189746.86223280002</v>
+      </c>
+      <c r="M19">
+        <v>119971.9242264</v>
+      </c>
+      <c r="N19">
+        <v>212982.19237920002</v>
+      </c>
+      <c r="O19">
+        <v>1.1385484366859957</v>
+      </c>
+      <c r="P19">
+        <v>1.5753294547410683</v>
+      </c>
+      <c r="Q19">
+        <v>1.461806150369562</v>
+      </c>
+      <c r="R19">
+        <v>1.6027161232820488</v>
+      </c>
+      <c r="S19">
+        <v>221.50281977290453</v>
+      </c>
+      <c r="T19">
+        <v>32.13122479133345</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20">
+      <c r="A20">
+        <v>1741972700</v>
+      </c>
+      <c r="B20">
+        <v>1.8234912745122036</v>
+      </c>
+      <c r="C20">
+        <v>18409.000442400007</v>
+      </c>
+      <c r="D20">
+        <v>126521.94311040001</v>
+      </c>
+      <c r="E20">
+        <v>302.65</v>
+      </c>
+      <c r="F20">
+        <v>297.85999999999996</v>
+      </c>
+      <c r="G20">
+        <v>110319.26481840001</v>
+      </c>
+      <c r="H20">
+        <v>209534.81401920004</v>
+      </c>
+      <c r="I20">
+        <v>92875.5303168</v>
+      </c>
+      <c r="J20">
+        <v>163753.6293984</v>
+      </c>
+      <c r="K20">
+        <v>135691.969548</v>
+      </c>
+      <c r="L20">
+        <v>214843.7766936</v>
+      </c>
+      <c r="M20">
+        <v>130245.1117392</v>
+      </c>
+      <c r="N20">
+        <v>257591.2683576</v>
+      </c>
+      <c r="O20">
+        <v>1.6044016840493662</v>
+      </c>
+      <c r="P20">
+        <v>1.2338959851459195</v>
+      </c>
+      <c r="Q20">
+        <v>1.5575519631040504</v>
+      </c>
+      <c r="R20">
+        <v>1.984110536608667</v>
+      </c>
+      <c r="S20">
+        <v>349.87610075703196</v>
+      </c>
+      <c r="T20">
+        <v>47.03568872538304</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20">
+      <c r="A21">
+        <v>1741972701</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>-34542.73116720002</v>
+      </c>
+      <c r="D21">
+        <v>82947.08064</v>
+      </c>
+      <c r="E21">
+        <v>303.14</v>
+      </c>
+      <c r="F21">
+        <v>295.5</v>
+      </c>
+      <c r="G21">
+        <v>101562.923784</v>
+      </c>
+      <c r="H21">
+        <v>237527.5263024</v>
+      </c>
+      <c r="I21">
+        <v>128176.6847232</v>
+      </c>
+      <c r="J21">
+        <v>252971.78135520002</v>
+      </c>
+      <c r="K21">
+        <v>74673.37257600001</v>
+      </c>
+      <c r="L21">
+        <v>152032.5429744</v>
+      </c>
+      <c r="M21">
+        <v>116317.7031648</v>
+      </c>
+      <c r="N21">
+        <v>245732.2867992</v>
+      </c>
+      <c r="O21">
+        <v>1.8532679853150253</v>
+      </c>
+      <c r="P21">
+        <v>1.9557777009714101</v>
+      </c>
+      <c r="Q21">
+        <v>1.1795040422691863</v>
+      </c>
+      <c r="R21">
+        <v>1.9121506532311674</v>
+      </c>
+      <c r="S21">
+        <v>690.0700381786789</v>
+      </c>
+      <c r="T21">
+        <v>44.99680413605927</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
function for excell calls
</commit_message>
<xml_diff>
--- a/src/monitoring_data.xlsx
+++ b/src/monitoring_data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="20">
   <si>
     <t>Time</t>
     <phoneticPr fontId="1"/>
@@ -28,15 +28,71 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>P, Pa</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Temp, K</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Temp2, K</t>
+    <t>P,Pa</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>t1ci</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>t2i</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>pstat1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ppito1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>pstat2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ppito2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>pstat3</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ppito3</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>pstat4</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ppito4</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>sflow1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>sflow2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>sflow3</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>sflow4</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>sflow_fract</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>sflow_uneven</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -341,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T21"/>
+  <dimension ref="A1:T18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -350,7 +406,7 @@
     <col min="1" max="20" width="8.38" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:20">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -369,1245 +425,1101 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="2" spans="1:20">
       <c r="A2">
-        <v>1741972681</v>
+        <v>1741982894</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>0.5619334366557527</v>
       </c>
       <c r="C2">
-        <v>-26406.918237599995</v>
+        <v>1999.4794488000043</v>
       </c>
       <c r="D2">
-        <v>92461.84491360001</v>
+        <v>94116.5865264</v>
       </c>
       <c r="E2">
-        <v>297.51</v>
+        <v>294.73999999999995</v>
       </c>
       <c r="F2">
-        <v>299.56</v>
+        <v>293.54999999999995</v>
       </c>
       <c r="G2">
-        <v>72053.3650224</v>
+        <v>135416.1792792</v>
       </c>
       <c r="H2">
-        <v>208500.60051120003</v>
+        <v>236700.15549600002</v>
       </c>
       <c r="I2">
-        <v>112663.48210319999</v>
+        <v>123074.56475040001</v>
       </c>
       <c r="J2">
-        <v>248076.504084</v>
+        <v>198710.04596880003</v>
       </c>
       <c r="K2">
-        <v>85015.507656</v>
+        <v>70329.6758424</v>
       </c>
       <c r="L2">
-        <v>209259.0237504</v>
+        <v>189057.3865608</v>
       </c>
       <c r="M2">
-        <v>73914.9493368</v>
+        <v>88669.72871760001</v>
       </c>
       <c r="N2">
-        <v>172096.2850296</v>
+        <v>177749.98554000002</v>
       </c>
       <c r="O2">
-        <v>1.5932451846147049</v>
+        <v>1.792356164580798</v>
       </c>
       <c r="P2">
-        <v>1.9211093235729242</v>
+        <v>1.4637610748565775</v>
       </c>
       <c r="Q2">
-        <v>1.6195926527992623</v>
+        <v>1.4700875131519855</v>
       </c>
       <c r="R2">
-        <v>1.3336656169424448</v>
+        <v>1.381355073691699</v>
       </c>
       <c r="S2">
-        <v>646.7612777929336</v>
+        <v>1086.8831480520398</v>
       </c>
       <c r="T2">
-        <v>36.33140862329453</v>
+        <v>26.91753188371865</v>
       </c>
     </row>
     <row r="3" spans="1:20">
       <c r="A3">
-        <v>1741972682</v>
+        <v>1741982895</v>
       </c>
       <c r="B3">
-        <v>0.809789441442755</v>
+        <v>1</v>
       </c>
       <c r="C3">
-        <v>4481.591867999989</v>
+        <v>-24614.281490399997</v>
       </c>
       <c r="D3">
-        <v>91841.3168088</v>
+        <v>70191.780708</v>
       </c>
       <c r="E3">
-        <v>302.85999999999996</v>
+        <v>300.15</v>
       </c>
       <c r="F3">
-        <v>300.39</v>
+        <v>294.75</v>
       </c>
       <c r="G3">
-        <v>130658.79714240001</v>
+        <v>103286.612964</v>
       </c>
       <c r="H3">
-        <v>233597.51497200003</v>
+        <v>222841.6944888</v>
       </c>
       <c r="I3">
-        <v>130107.2166048</v>
+        <v>100459.7627088</v>
       </c>
       <c r="J3">
-        <v>257729.16349200002</v>
+        <v>171889.442328</v>
       </c>
       <c r="K3">
-        <v>126590.8906776</v>
+        <v>75776.5336512</v>
       </c>
       <c r="L3">
-        <v>230012.2414776</v>
+        <v>204087.9562104</v>
       </c>
       <c r="M3">
-        <v>121281.9280032</v>
+        <v>77913.9082344</v>
       </c>
       <c r="N3">
-        <v>255522.8413416</v>
+        <v>154652.550528</v>
       </c>
       <c r="O3">
-        <v>1.7590054195874076</v>
+        <v>1.738292841661442</v>
       </c>
       <c r="P3">
-        <v>1.977187853115395</v>
+        <v>1.2907461697502303</v>
       </c>
       <c r="Q3">
-        <v>1.7386002983993725</v>
+        <v>1.5834767800619105</v>
       </c>
       <c r="R3">
-        <v>1.9717302331031612</v>
+        <v>1.1980234690375042</v>
       </c>
       <c r="S3">
-        <v>919.5629657677797</v>
+        <v>581.0539260511086</v>
       </c>
       <c r="T3">
-        <v>12.816050065201326</v>
+        <v>37.19237395369851</v>
       </c>
     </row>
     <row r="4" spans="1:20">
       <c r="A4">
-        <v>1741972683</v>
+        <v>1741982896</v>
       </c>
       <c r="B4">
-        <v>2.6013627227135028</v>
+        <v>1.6065185386028829</v>
       </c>
       <c r="C4">
-        <v>56468.0575368</v>
+        <v>21166.903130399995</v>
       </c>
       <c r="D4">
-        <v>129900.3739032</v>
+        <v>93909.7438248</v>
       </c>
       <c r="E4">
-        <v>296.78</v>
+        <v>298.53</v>
       </c>
       <c r="F4">
-        <v>296.04999999999995</v>
+        <v>296.37</v>
       </c>
       <c r="G4">
-        <v>90876.050868</v>
+        <v>127969.84202160001</v>
       </c>
       <c r="H4">
-        <v>168511.0115352</v>
+        <v>243663.85978320002</v>
       </c>
       <c r="I4">
-        <v>80258.1255192</v>
+        <v>81843.9195648</v>
       </c>
       <c r="J4">
-        <v>150929.3818992</v>
+        <v>200778.4729848</v>
       </c>
       <c r="K4">
-        <v>101907.66162</v>
+        <v>123557.1977208</v>
       </c>
       <c r="L4">
-        <v>223531.17016080001</v>
+        <v>204846.3794496</v>
       </c>
       <c r="M4">
-        <v>132451.4338896</v>
+        <v>91910.264376</v>
       </c>
       <c r="N4">
-        <v>224289.5934</v>
+        <v>221600.6382792</v>
       </c>
       <c r="O4">
-        <v>1.288541551877632</v>
+        <v>1.8711896809493112</v>
       </c>
       <c r="P4">
-        <v>1.15717487748923</v>
+        <v>1.5624967669163048</v>
       </c>
       <c r="Q4">
-        <v>1.7410343736230252</v>
+        <v>1.5175983110435871</v>
       </c>
       <c r="R4">
-        <v>1.674913207280861</v>
+        <v>1.7255050886551566</v>
       </c>
       <c r="S4">
-        <v>225.3305146218286</v>
+        <v>415.60615001497985</v>
       </c>
       <c r="T4">
-        <v>39.84257679121576</v>
+        <v>21.18331581364427</v>
       </c>
     </row>
     <row r="5" spans="1:20">
       <c r="A5">
-        <v>1741972684</v>
+        <v>1741982897</v>
       </c>
       <c r="B5">
-        <v>2.3011754155793462</v>
+        <v>1.7602844368955317</v>
       </c>
       <c r="C5">
-        <v>38748.53276640001</v>
+        <v>17443.734501600004</v>
       </c>
       <c r="D5">
-        <v>120937.19016720001</v>
+        <v>121557.71827200001</v>
       </c>
       <c r="E5">
-        <v>297.34999999999997</v>
+        <v>296.22999999999996</v>
       </c>
       <c r="F5">
-        <v>301.2</v>
+        <v>302.66999999999996</v>
       </c>
       <c r="G5">
-        <v>76259.1666216</v>
+        <v>107975.04753360001</v>
       </c>
       <c r="H5">
-        <v>212499.55940880004</v>
+        <v>218429.05018800002</v>
       </c>
       <c r="I5">
-        <v>105010.302144</v>
+        <v>124453.51609440001</v>
       </c>
       <c r="J5">
-        <v>220566.42477120002</v>
+        <v>258694.42943279998</v>
       </c>
       <c r="K5">
-        <v>92668.6876152</v>
+        <v>98046.5978568</v>
       </c>
       <c r="L5">
-        <v>203053.74270240002</v>
+        <v>214567.9864248</v>
       </c>
       <c r="M5">
-        <v>82188.6574008</v>
+        <v>128314.5798576</v>
       </c>
       <c r="N5">
-        <v>206018.488092</v>
+        <v>228564.3425664</v>
       </c>
       <c r="O5">
-        <v>1.6259081290945516</v>
+        <v>1.6733548984345525</v>
       </c>
       <c r="P5">
-        <v>1.6993452408145833</v>
+        <v>1.9867174445328664</v>
       </c>
       <c r="Q5">
-        <v>1.567902782705729</v>
+        <v>1.652707194399507</v>
       </c>
       <c r="R5">
-        <v>1.5888880910669267</v>
+        <v>1.7130418691120655</v>
       </c>
       <c r="S5">
-        <v>281.6840558871461</v>
+        <v>399.1298939658782</v>
       </c>
       <c r="T5">
-        <v>8.111173152634647</v>
+        <v>19.01615374540238</v>
       </c>
     </row>
     <row r="6" spans="1:20">
       <c r="A6">
-        <v>1741972685</v>
+        <v>1741982898</v>
       </c>
       <c r="B6">
-        <v>2.646460932002791</v>
+        <v>1</v>
       </c>
       <c r="C6">
-        <v>46608.555427200015</v>
+        <v>-12134.771827200006</v>
       </c>
       <c r="D6">
-        <v>137829.34413120002</v>
+        <v>102183.4518888</v>
       </c>
       <c r="E6">
-        <v>299.46999999999997</v>
+        <v>296.72999999999996</v>
       </c>
       <c r="F6">
-        <v>299.53999999999996</v>
+        <v>293.29999999999995</v>
       </c>
       <c r="G6">
-        <v>75431.7958152</v>
+        <v>78948.1217424</v>
       </c>
       <c r="H6">
-        <v>176302.08662880003</v>
+        <v>161064.67427760002</v>
       </c>
       <c r="I6">
-        <v>69364.4099016</v>
+        <v>98115.545424</v>
       </c>
       <c r="J6">
-        <v>142586.726268</v>
+        <v>179749.4649888</v>
       </c>
       <c r="K6">
-        <v>112801.3772376</v>
+        <v>117696.6545088</v>
       </c>
       <c r="L6">
-        <v>218773.788024</v>
+        <v>192228.974652</v>
       </c>
       <c r="M6">
-        <v>72260.20772399999</v>
+        <v>107768.204832</v>
       </c>
       <c r="N6">
-        <v>152308.33324319997</v>
+        <v>230356.97931360002</v>
       </c>
       <c r="O6">
-        <v>1.3662665484510854</v>
+        <v>1.2545022566349358</v>
       </c>
       <c r="P6">
-        <v>1.0997170440384454</v>
+        <v>1.3774819688211855</v>
       </c>
       <c r="Q6">
-        <v>1.675939968529213</v>
+        <v>1.4233415368878546</v>
       </c>
       <c r="R6">
-        <v>1.1769812438130236</v>
+        <v>1.80048751710005</v>
       </c>
       <c r="S6">
-        <v>200.98179952373306</v>
+        <v>585.5813279444027</v>
       </c>
       <c r="T6">
-        <v>43.333952806774704</v>
+        <v>37.295264340597434</v>
       </c>
     </row>
     <row r="7" spans="1:20">
       <c r="A7">
-        <v>1741972686</v>
+        <v>1741982899</v>
       </c>
       <c r="B7">
-        <v>2.707664209526076</v>
+        <v>0.8776581770463965</v>
       </c>
       <c r="C7">
-        <v>53365.4170128</v>
+        <v>5998.438346399998</v>
       </c>
       <c r="D7">
-        <v>136933.0257576</v>
+        <v>80396.0206536</v>
       </c>
       <c r="E7">
-        <v>297.33</v>
+        <v>293.21</v>
       </c>
       <c r="F7">
-        <v>299.46</v>
+        <v>297.60999999999996</v>
       </c>
       <c r="G7">
-        <v>118386.13018080001</v>
+        <v>88669.72871760001</v>
       </c>
       <c r="H7">
-        <v>232218.56362800003</v>
+        <v>224082.75069840002</v>
       </c>
       <c r="I7">
-        <v>135829.86468240002</v>
+        <v>117903.4972104</v>
       </c>
       <c r="J7">
-        <v>249110.71759200003</v>
+        <v>198227.41299840002</v>
       </c>
       <c r="K7">
-        <v>93771.8486904</v>
+        <v>74949.1628448</v>
       </c>
       <c r="L7">
-        <v>183610.528752</v>
+        <v>155479.92133440002</v>
       </c>
       <c r="M7">
-        <v>121144.0328688</v>
+        <v>102459.2421576</v>
       </c>
       <c r="N7">
-        <v>213533.7729168</v>
+        <v>198296.3605656</v>
       </c>
       <c r="O7">
-        <v>1.7819896445511718</v>
+        <v>1.737873280108273</v>
       </c>
       <c r="P7">
-        <v>1.8897164960047375</v>
+        <v>1.4728333758181598</v>
       </c>
       <c r="Q7">
-        <v>1.4086461705702784</v>
+        <v>1.2039677274422733</v>
       </c>
       <c r="R7">
-        <v>1.6045657402887512</v>
+        <v>1.5235151841765324</v>
       </c>
       <c r="S7">
-        <v>246.88874004007326</v>
+        <v>676.5947977069121</v>
       </c>
       <c r="T7">
-        <v>28.785413477589906</v>
+        <v>35.96419727548095</v>
       </c>
     </row>
     <row r="8" spans="1:20">
       <c r="A8">
-        <v>1741972688</v>
+        <v>1741982900</v>
       </c>
       <c r="B8">
-        <v>0.4022693008879437</v>
+        <v>1</v>
       </c>
       <c r="C8">
-        <v>827.3708063999802</v>
+        <v>-15306.35991839999</v>
       </c>
       <c r="D8">
-        <v>117696.6545088</v>
+        <v>87290.77737360001</v>
       </c>
       <c r="E8">
-        <v>300.14</v>
+        <v>299.92999999999995</v>
       </c>
       <c r="F8">
-        <v>301.69</v>
+        <v>300.71</v>
       </c>
       <c r="G8">
-        <v>81981.8146992</v>
+        <v>78189.69850320001</v>
       </c>
       <c r="H8">
-        <v>203743.2183744</v>
+        <v>169338.38234160002</v>
       </c>
       <c r="I8">
-        <v>115972.9653288</v>
+        <v>101838.7140528</v>
       </c>
       <c r="J8">
-        <v>186851.0644104</v>
+        <v>203674.2708072</v>
       </c>
       <c r="K8">
-        <v>130107.2166048</v>
+        <v>81085.4963256</v>
       </c>
       <c r="L8">
-        <v>250696.51163760002</v>
+        <v>186644.2217088</v>
       </c>
       <c r="M8">
-        <v>118317.1826136</v>
+        <v>88118.14818</v>
       </c>
       <c r="N8">
-        <v>249248.6127264</v>
+        <v>173613.13150800002</v>
       </c>
       <c r="O8">
-        <v>1.5706939525080004</v>
+        <v>1.308011854712848</v>
       </c>
       <c r="P8">
-        <v>1.35649662802757</v>
+        <v>1.5634522687803507</v>
       </c>
       <c r="Q8">
-        <v>1.911768132729978</v>
+        <v>1.443674688028595</v>
       </c>
       <c r="R8">
-        <v>1.9191526522384403</v>
+        <v>1.3302676196792895</v>
       </c>
       <c r="S8">
-        <v>1679.996795824728</v>
+        <v>564.5406431201084</v>
       </c>
       <c r="T8">
-        <v>33.30256006628621</v>
+        <v>18.09899196314598</v>
       </c>
     </row>
     <row r="9" spans="1:20">
       <c r="A9">
-        <v>1741972689</v>
+        <v>1741982901</v>
       </c>
       <c r="B9">
-        <v>0.26007318202771706</v>
+        <v>2.655499473404385</v>
       </c>
       <c r="C9">
-        <v>482.63297040000907</v>
+        <v>50124.8813544</v>
       </c>
       <c r="D9">
-        <v>84532.8746856</v>
+        <v>134657.75604</v>
       </c>
       <c r="E9">
-        <v>296.4</v>
+        <v>294.58</v>
       </c>
       <c r="F9">
-        <v>297.45</v>
+        <v>301.28</v>
       </c>
       <c r="G9">
-        <v>91772.3692416</v>
+        <v>88393.93844879999</v>
       </c>
       <c r="H9">
-        <v>224013.80313120002</v>
+        <v>223462.2225936</v>
       </c>
       <c r="I9">
-        <v>107285.5718616</v>
+        <v>131348.2728144</v>
       </c>
       <c r="J9">
-        <v>244146.4927536</v>
+        <v>215809.04263440002</v>
       </c>
       <c r="K9">
-        <v>134381.96577120002</v>
+        <v>92323.9497792</v>
       </c>
       <c r="L9">
-        <v>215326.40966400004</v>
+        <v>206432.1734952</v>
       </c>
       <c r="M9">
-        <v>83291.81847600001</v>
+        <v>97357.1221848</v>
       </c>
       <c r="N9">
-        <v>153342.54675120002</v>
+        <v>221807.4809808</v>
       </c>
       <c r="O9">
-        <v>1.7404622947932127</v>
+        <v>1.7224414331774929</v>
       </c>
       <c r="P9">
-        <v>1.898655778661568</v>
+        <v>1.580333913764304</v>
       </c>
       <c r="Q9">
-        <v>1.5705877823092909</v>
+        <v>1.5947008427906741</v>
       </c>
       <c r="R9">
-        <v>1.1680931109439254</v>
+        <v>1.7139498361625278</v>
       </c>
       <c r="S9">
-        <v>2452.3093526914627</v>
+        <v>248.9710915822199</v>
       </c>
       <c r="T9">
-        <v>45.819109164849344</v>
+        <v>8.597692470979531</v>
       </c>
     </row>
     <row r="10" spans="1:20">
       <c r="A10">
-        <v>1741972690</v>
+        <v>1741982902</v>
       </c>
       <c r="B10">
         <v>1</v>
       </c>
       <c r="C10">
-        <v>-14272.14641039999</v>
+        <v>-36886.948452</v>
       </c>
       <c r="D10">
-        <v>85911.82602960001</v>
+        <v>74259.68717280001</v>
       </c>
       <c r="E10">
-        <v>302.96</v>
+        <v>300.94</v>
       </c>
       <c r="F10">
-        <v>294.34999999999997</v>
+        <v>297.28999999999996</v>
       </c>
       <c r="G10">
-        <v>133554.5949648</v>
+        <v>89290.2568224</v>
       </c>
       <c r="H10">
-        <v>261314.4369864</v>
+        <v>184437.8995584</v>
       </c>
       <c r="I10">
-        <v>102252.39945600001</v>
+        <v>81016.54875840001</v>
       </c>
       <c r="J10">
-        <v>234218.04307680004</v>
+        <v>168442.063968</v>
       </c>
       <c r="K10">
-        <v>129073.00309680002</v>
+        <v>108388.7329368</v>
       </c>
       <c r="L10">
-        <v>252764.93865360005</v>
+        <v>243112.2792456</v>
       </c>
       <c r="M10">
-        <v>133830.3852336</v>
+        <v>104941.3545768</v>
       </c>
       <c r="N10">
-        <v>262279.7029272</v>
+        <v>214292.19615600002</v>
       </c>
       <c r="O10">
-        <v>2.0219085820960307</v>
+        <v>1.428469709963884</v>
       </c>
       <c r="P10">
-        <v>1.8310936630144394</v>
+        <v>1.305274152268579</v>
       </c>
       <c r="Q10">
-        <v>1.9559880510317982</v>
+        <v>1.8907372583171451</v>
       </c>
       <c r="R10">
-        <v>2.0298243263295794</v>
+        <v>1.657988471250528</v>
       </c>
       <c r="S10">
-        <v>783.8814622471848</v>
+        <v>628.2469591800136</v>
       </c>
       <c r="T10">
-        <v>10.140852814425832</v>
+        <v>37.27598502427843</v>
       </c>
     </row>
     <row r="11" spans="1:20">
       <c r="A11">
-        <v>1741972691</v>
+        <v>1741982903</v>
       </c>
       <c r="B11">
-        <v>0.2568514408351907</v>
+        <v>1</v>
       </c>
       <c r="C11">
-        <v>482.63297039997997</v>
+        <v>-12617.404797600015</v>
       </c>
       <c r="D11">
-        <v>83774.4514464</v>
+        <v>104872.4070096</v>
       </c>
       <c r="E11">
-        <v>301.19</v>
+        <v>301.98999999999995</v>
       </c>
       <c r="F11">
-        <v>296.02</v>
+        <v>298.09999999999997</v>
       </c>
       <c r="G11">
-        <v>111905.058864</v>
+        <v>101287.13351520001</v>
       </c>
       <c r="H11">
-        <v>191539.49898000003</v>
+        <v>187954.2254856</v>
       </c>
       <c r="I11">
-        <v>129417.74093279999</v>
+        <v>94806.0621984</v>
       </c>
       <c r="J11">
-        <v>212844.2972448</v>
+        <v>186782.1168432</v>
       </c>
       <c r="K11">
-        <v>122454.0366456</v>
+        <v>133140.9095616</v>
       </c>
       <c r="L11">
-        <v>240147.533856</v>
+        <v>225737.4923112</v>
       </c>
       <c r="M11">
-        <v>104045.03620320001</v>
+        <v>82602.342804</v>
       </c>
       <c r="N11">
-        <v>218980.63072560003</v>
+        <v>163822.57696560002</v>
       </c>
       <c r="O11">
-        <v>1.4353700573466364</v>
+        <v>1.4324739283152899</v>
       </c>
       <c r="P11">
-        <v>1.5730016450335857</v>
+        <v>1.4374156172575006</v>
       </c>
       <c r="Q11">
-        <v>1.8534593041589964</v>
+        <v>1.6806090894813481</v>
       </c>
       <c r="R11">
-        <v>1.7020616844314516</v>
+        <v>1.2617805764936645</v>
       </c>
       <c r="S11">
-        <v>2555.5210707120023</v>
+        <v>581.2279211547802</v>
       </c>
       <c r="T11">
-        <v>25.47812808624895</v>
+        <v>28.8237022168899</v>
       </c>
     </row>
     <row r="12" spans="1:20">
       <c r="A12">
-        <v>1741972692</v>
+        <v>1741982904</v>
       </c>
       <c r="B12">
-        <v>2.6539058333361734</v>
+        <v>2.3655113748635053</v>
       </c>
       <c r="C12">
-        <v>46263.817591200015</v>
+        <v>41575.383021600006</v>
       </c>
       <c r="D12">
-        <v>137691.44899680003</v>
+        <v>122936.66961600001</v>
       </c>
       <c r="E12">
-        <v>296.29999999999995</v>
+        <v>298.07</v>
       </c>
       <c r="F12">
-        <v>300.92999999999995</v>
+        <v>294.96</v>
       </c>
       <c r="G12">
-        <v>111698.21616240001</v>
+        <v>99839.234604</v>
       </c>
       <c r="H12">
-        <v>236424.36522720003</v>
+        <v>212016.9264384</v>
       </c>
       <c r="I12">
-        <v>119489.29125600001</v>
+        <v>88531.8335832</v>
       </c>
       <c r="J12">
-        <v>208500.60051120003</v>
+        <v>162443.62562160002</v>
       </c>
       <c r="K12">
-        <v>83636.556312</v>
+        <v>119213.50098720002</v>
       </c>
       <c r="L12">
-        <v>194159.5065336</v>
+        <v>240974.90466240002</v>
       </c>
       <c r="M12">
-        <v>73777.0542024</v>
+        <v>131693.0106504</v>
       </c>
       <c r="N12">
-        <v>196779.5140872</v>
+        <v>228495.3949992</v>
       </c>
       <c r="O12">
-        <v>1.8232713696112575</v>
+        <v>1.6518439426417242</v>
       </c>
       <c r="P12">
-        <v>1.5585860807062293</v>
+        <v>1.2417619318980622</v>
       </c>
       <c r="Q12">
-        <v>1.5012385781459003</v>
+        <v>1.8698952784423584</v>
       </c>
       <c r="R12">
-        <v>1.5122194703104306</v>
+        <v>1.722447102281079</v>
       </c>
       <c r="S12">
-        <v>240.97748376906014</v>
+        <v>274.1879969035227</v>
       </c>
       <c r="T12">
-        <v>20.14179231827427</v>
+        <v>38.738104087375525</v>
       </c>
     </row>
     <row r="13" spans="1:20">
       <c r="A13">
-        <v>1741972693</v>
+        <v>1741982905</v>
       </c>
       <c r="B13">
-        <v>2.2869915237286373</v>
+        <v>1</v>
       </c>
       <c r="C13">
-        <v>42954.33436559999</v>
+        <v>-551.5805376000062</v>
       </c>
       <c r="D13">
-        <v>116110.86046319999</v>
+        <v>79154.964444</v>
       </c>
       <c r="E13">
-        <v>294.51</v>
+        <v>298.77</v>
       </c>
       <c r="F13">
-        <v>294.75</v>
+        <v>300.32</v>
       </c>
       <c r="G13">
-        <v>130176.16417200002</v>
+        <v>133968.280368</v>
       </c>
       <c r="H13">
-        <v>199744.25947680004</v>
+        <v>256005.474312</v>
       </c>
       <c r="I13">
-        <v>111215.58319200002</v>
+        <v>129555.63606720002</v>
       </c>
       <c r="J13">
-        <v>248765.97975600002</v>
+        <v>241043.85222960002</v>
       </c>
       <c r="K13">
-        <v>74880.2152776</v>
+        <v>87221.8298064</v>
       </c>
       <c r="L13">
-        <v>147550.9511064</v>
+        <v>180438.9406608</v>
       </c>
       <c r="M13">
-        <v>127625.10418560001</v>
+        <v>71294.9417832</v>
       </c>
       <c r="N13">
-        <v>240078.5862888</v>
+        <v>173888.9217768</v>
       </c>
       <c r="O13">
-        <v>1.432884755850862</v>
+        <v>1.9541488310613804</v>
       </c>
       <c r="P13">
-        <v>1.9429181536016813</v>
+        <v>1.8312284062539779</v>
       </c>
       <c r="Q13">
-        <v>1.1419654098258059</v>
+        <v>1.390606408601513</v>
       </c>
       <c r="R13">
-        <v>1.8448377466954398</v>
+        <v>1.3445859721225242</v>
       </c>
       <c r="S13">
-        <v>278.20855477419525</v>
+        <v>652.0569618039394</v>
       </c>
       <c r="T13">
-        <v>50.35375350733996</v>
+        <v>37.393227564197964</v>
       </c>
     </row>
     <row r="14" spans="1:20">
       <c r="A14">
-        <v>1741972694</v>
+        <v>1741982906</v>
       </c>
       <c r="B14">
-        <v>1.557549234531337</v>
+        <v>2.330246070350973</v>
       </c>
       <c r="C14">
-        <v>12272.66696159997</v>
+        <v>39506.95600560002</v>
       </c>
       <c r="D14">
-        <v>128797.21282799999</v>
+        <v>123281.40745200001</v>
       </c>
       <c r="E14">
-        <v>299.29999999999995</v>
+        <v>301.46</v>
       </c>
       <c r="F14">
-        <v>300.51</v>
+        <v>300.38</v>
       </c>
       <c r="G14">
-        <v>113284.01020799999</v>
+        <v>108526.62807120002</v>
       </c>
       <c r="H14">
-        <v>248559.1370544</v>
+        <v>218704.8404568</v>
       </c>
       <c r="I14">
-        <v>126039.31014</v>
+        <v>92117.1070776</v>
       </c>
       <c r="J14">
-        <v>219463.263696</v>
+        <v>225116.9642064</v>
       </c>
       <c r="K14">
-        <v>78603.38390639999</v>
+        <v>103079.77026240001</v>
       </c>
       <c r="L14">
-        <v>205260.0648528</v>
+        <v>187264.74981360004</v>
       </c>
       <c r="M14">
-        <v>98873.96866320001</v>
+        <v>129210.89823120002</v>
       </c>
       <c r="N14">
-        <v>235459.0992864</v>
+        <v>230219.08417920003</v>
       </c>
       <c r="O14">
-        <v>1.9215718264540562</v>
+        <v>1.6811644204954457</v>
       </c>
       <c r="P14">
-        <v>1.640690652000439</v>
+        <v>1.740411644478671</v>
       </c>
       <c r="Q14">
-        <v>1.5809962386198093</v>
+        <v>1.4154589918426652</v>
       </c>
       <c r="R14">
-        <v>1.8212753193206022</v>
+        <v>1.7321184029449719</v>
       </c>
       <c r="S14">
-        <v>447.1469589525058</v>
+        <v>281.90814452365254</v>
       </c>
       <c r="T14">
-        <v>19.560567070502312</v>
+        <v>19.78657704536505</v>
       </c>
     </row>
     <row r="15" spans="1:20">
       <c r="A15">
-        <v>1741972695</v>
+        <v>1741982907</v>
       </c>
       <c r="B15">
-        <v>1</v>
+        <v>1.0435600316301903</v>
       </c>
       <c r="C15">
-        <v>-38334.84736319998</v>
+        <v>8066.8653624</v>
       </c>
       <c r="D15">
-        <v>93427.1108544</v>
+        <v>87428.672508</v>
       </c>
       <c r="E15">
-        <v>297.02</v>
+        <v>297.65</v>
       </c>
       <c r="F15">
-        <v>299.03999999999996</v>
+        <v>302.08</v>
       </c>
       <c r="G15">
-        <v>98184.49299120001</v>
+        <v>108802.41834</v>
       </c>
       <c r="H15">
-        <v>209259.0237504</v>
+        <v>243939.650052</v>
       </c>
       <c r="I15">
-        <v>95357.64273600001</v>
+        <v>79499.70228</v>
       </c>
       <c r="J15">
-        <v>186713.169276</v>
+        <v>186851.0644104</v>
       </c>
       <c r="K15">
-        <v>93565.0059888</v>
+        <v>123488.2501536</v>
       </c>
       <c r="L15">
-        <v>217532.7318144</v>
+        <v>211327.45076640003</v>
       </c>
       <c r="M15">
-        <v>70812.30881280001</v>
+        <v>111284.5307592</v>
       </c>
       <c r="N15">
-        <v>204294.798912</v>
+        <v>203329.5329712</v>
       </c>
       <c r="O15">
-        <v>1.619543413646154</v>
+        <v>1.8820554232956184</v>
       </c>
       <c r="P15">
-        <v>1.4334524413814993</v>
+        <v>1.4418341068101945</v>
       </c>
       <c r="Q15">
-        <v>1.6872553175223082</v>
+        <v>1.5676042824382892</v>
       </c>
       <c r="R15">
-        <v>1.562996632228709</v>
+        <v>1.5344884677307642</v>
       </c>
       <c r="S15">
-        <v>630.3247804778671</v>
+        <v>615.775047482085</v>
       </c>
       <c r="T15">
-        <v>16.106165202541693</v>
+        <v>27.40258514790637</v>
       </c>
     </row>
     <row r="16" spans="1:20">
       <c r="A16">
-        <v>1741972696</v>
+        <v>1741982908</v>
       </c>
       <c r="B16">
         <v>1</v>
       </c>
       <c r="C16">
-        <v>-3792.1161960000027</v>
+        <v>-9307.921572000007</v>
       </c>
       <c r="D16">
-        <v>108664.52320560001</v>
+        <v>81154.4438928</v>
       </c>
       <c r="E16">
-        <v>294.73999999999995</v>
+        <v>300.35999999999996</v>
       </c>
       <c r="F16">
-        <v>298.98999999999995</v>
+        <v>295.96999999999997</v>
       </c>
       <c r="G16">
-        <v>92875.5303168</v>
+        <v>106320.3059208</v>
       </c>
       <c r="H16">
-        <v>172372.0752984</v>
+        <v>198710.04596880003</v>
       </c>
       <c r="I16">
-        <v>81568.12929600001</v>
+        <v>121488.7707048</v>
       </c>
       <c r="J16">
-        <v>162443.62562160002</v>
+        <v>223255.379892</v>
       </c>
       <c r="K16">
-        <v>115490.3323584</v>
+        <v>77431.275264</v>
       </c>
       <c r="L16">
-        <v>236906.9981976</v>
+        <v>153480.44188559998</v>
       </c>
       <c r="M16">
-        <v>113490.8529096</v>
+        <v>120316.66206240002</v>
       </c>
       <c r="N16">
-        <v>198434.2557</v>
+        <v>242560.698708</v>
       </c>
       <c r="O16">
-        <v>1.311799737186064</v>
+        <v>1.5219814957366056</v>
       </c>
       <c r="P16">
-        <v>1.2499207169496094</v>
+        <v>1.7042550120224853</v>
       </c>
       <c r="Q16">
-        <v>1.8285100999227988</v>
+        <v>1.186288144349866</v>
       </c>
       <c r="R16">
-        <v>1.488986736635078</v>
+        <v>1.878461579300712</v>
       </c>
       <c r="S16">
-        <v>587.921729069355</v>
+        <v>629.0986231409669</v>
       </c>
       <c r="T16">
-        <v>39.365062005043555</v>
+        <v>44.010487989622916</v>
       </c>
     </row>
     <row r="17" spans="1:20">
       <c r="A17">
-        <v>1741972697</v>
+        <v>1741982910</v>
       </c>
       <c r="B17">
-        <v>1</v>
+        <v>1.944483825021536</v>
       </c>
       <c r="C17">
-        <v>-35990.630078400005</v>
+        <v>19029.528547200025</v>
       </c>
       <c r="D17">
-        <v>72673.8931272</v>
+        <v>135760.91711520002</v>
       </c>
       <c r="E17">
-        <v>295.96</v>
+        <v>297.2</v>
       </c>
       <c r="F17">
-        <v>299.46</v>
+        <v>302.15</v>
       </c>
       <c r="G17">
-        <v>81499.1817288</v>
+        <v>82947.08064</v>
       </c>
       <c r="H17">
-        <v>216981.1512768</v>
+        <v>188023.1730528</v>
       </c>
       <c r="I17">
-        <v>122867.7220488</v>
+        <v>84463.92711840001</v>
       </c>
       <c r="J17">
-        <v>210224.2896912</v>
+        <v>197606.8848936</v>
       </c>
       <c r="K17">
-        <v>82533.3952368</v>
+        <v>88393.93844879999</v>
       </c>
       <c r="L17">
-        <v>195193.7200416</v>
+        <v>204019.00864319998</v>
       </c>
       <c r="M17">
-        <v>71984.4174552</v>
+        <v>81637.07686320001</v>
       </c>
       <c r="N17">
-        <v>191056.8660096</v>
+        <v>185403.16549920003</v>
       </c>
       <c r="O17">
-        <v>1.6717948175833253</v>
+        <v>1.4507251257717741</v>
       </c>
       <c r="P17">
-        <v>1.5661316911939371</v>
+        <v>1.5247282107681932</v>
       </c>
       <c r="Q17">
-        <v>1.512654123452704</v>
+        <v>1.5743044058618914</v>
       </c>
       <c r="R17">
-        <v>1.4724101846716164</v>
+        <v>1.4305399548974267</v>
       </c>
       <c r="S17">
-        <v>622.2990816901583</v>
+        <v>307.5519384807971</v>
       </c>
       <c r="T17">
-        <v>12.81600045882646</v>
+        <v>9.615872536204275</v>
       </c>
     </row>
     <row r="18" spans="1:20">
       <c r="A18">
-        <v>1741972698</v>
+        <v>1741982911</v>
       </c>
       <c r="B18">
-        <v>2.10941970396002</v>
+        <v>1</v>
       </c>
       <c r="C18">
-        <v>30612.71983680001</v>
+        <v>-24407.438788800006</v>
       </c>
       <c r="D18">
-        <v>116869.28370240002</v>
+        <v>75914.4287856</v>
       </c>
       <c r="E18">
-        <v>295.83</v>
+        <v>298.78999999999996</v>
       </c>
       <c r="F18">
-        <v>297</v>
+        <v>302.97999999999996</v>
       </c>
       <c r="G18">
-        <v>107699.2572648</v>
+        <v>91496.57897280001</v>
       </c>
       <c r="H18">
-        <v>239182.26791520003</v>
+        <v>191953.18438320002</v>
       </c>
       <c r="I18">
-        <v>130245.1117392</v>
+        <v>106320.3059208</v>
       </c>
       <c r="J18">
-        <v>242560.698708</v>
+        <v>228978.0279696</v>
       </c>
       <c r="K18">
-        <v>74328.63474000001</v>
+        <v>90393.41789760001</v>
       </c>
       <c r="L18">
-        <v>162236.78292000003</v>
+        <v>160099.4083368</v>
       </c>
       <c r="M18">
-        <v>73570.21150080001</v>
+        <v>70398.6234096</v>
       </c>
       <c r="N18">
-        <v>195469.51031040002</v>
+        <v>179749.4649888</v>
       </c>
       <c r="O18">
-        <v>1.8606635355051766</v>
+        <v>1.474421695267795</v>
       </c>
       <c r="P18">
-        <v>1.8533682740325081</v>
+        <v>1.7615806778844048</v>
       </c>
       <c r="Q18">
-        <v>1.261372878237543</v>
+        <v>1.1975483285013906</v>
       </c>
       <c r="R18">
-        <v>1.5125201143929012</v>
+        <v>1.3808411645090097</v>
       </c>
       <c r="S18">
-        <v>307.5691760150115</v>
+        <v>581.43918661626</v>
       </c>
       <c r="T18">
-        <v>36.94806432203796</v>
-      </c>
-    </row>
-    <row r="19" spans="1:20">
-      <c r="A19">
-        <v>1741972699</v>
-      </c>
-      <c r="B19">
-        <v>2.6087253295479362</v>
-      </c>
-      <c r="C19">
-        <v>47435.926233599996</v>
-      </c>
-      <c r="D19">
-        <v>135485.1268464</v>
-      </c>
-      <c r="E19">
-        <v>302.2</v>
-      </c>
-      <c r="F19">
-        <v>299.71999999999997</v>
-      </c>
-      <c r="G19">
-        <v>80602.86335520001</v>
-      </c>
-      <c r="H19">
-        <v>149757.27325680002</v>
-      </c>
-      <c r="I19">
-        <v>88324.9908816</v>
-      </c>
-      <c r="J19">
-        <v>203329.5329712</v>
-      </c>
-      <c r="K19">
-        <v>71570.732052</v>
-      </c>
-      <c r="L19">
-        <v>189746.86223280002</v>
-      </c>
-      <c r="M19">
-        <v>119971.9242264</v>
-      </c>
-      <c r="N19">
-        <v>212982.19237920002</v>
-      </c>
-      <c r="O19">
-        <v>1.1385484366859957</v>
-      </c>
-      <c r="P19">
-        <v>1.5753294547410683</v>
-      </c>
-      <c r="Q19">
-        <v>1.461806150369562</v>
-      </c>
-      <c r="R19">
-        <v>1.6027161232820488</v>
-      </c>
-      <c r="S19">
-        <v>221.50281977290453</v>
-      </c>
-      <c r="T19">
-        <v>32.13122479133345</v>
-      </c>
-    </row>
-    <row r="20" spans="1:20">
-      <c r="A20">
-        <v>1741972700</v>
-      </c>
-      <c r="B20">
-        <v>1.8234912745122036</v>
-      </c>
-      <c r="C20">
-        <v>18409.000442400007</v>
-      </c>
-      <c r="D20">
-        <v>126521.94311040001</v>
-      </c>
-      <c r="E20">
-        <v>302.65</v>
-      </c>
-      <c r="F20">
-        <v>297.85999999999996</v>
-      </c>
-      <c r="G20">
-        <v>110319.26481840001</v>
-      </c>
-      <c r="H20">
-        <v>209534.81401920004</v>
-      </c>
-      <c r="I20">
-        <v>92875.5303168</v>
-      </c>
-      <c r="J20">
-        <v>163753.6293984</v>
-      </c>
-      <c r="K20">
-        <v>135691.969548</v>
-      </c>
-      <c r="L20">
-        <v>214843.7766936</v>
-      </c>
-      <c r="M20">
-        <v>130245.1117392</v>
-      </c>
-      <c r="N20">
-        <v>257591.2683576</v>
-      </c>
-      <c r="O20">
-        <v>1.6044016840493662</v>
-      </c>
-      <c r="P20">
-        <v>1.2338959851459195</v>
-      </c>
-      <c r="Q20">
-        <v>1.5575519631040504</v>
-      </c>
-      <c r="R20">
-        <v>1.984110536608667</v>
-      </c>
-      <c r="S20">
-        <v>349.87610075703196</v>
-      </c>
-      <c r="T20">
-        <v>47.03568872538304</v>
-      </c>
-    </row>
-    <row r="21" spans="1:20">
-      <c r="A21">
-        <v>1741972701</v>
-      </c>
-      <c r="B21">
-        <v>1</v>
-      </c>
-      <c r="C21">
-        <v>-34542.73116720002</v>
-      </c>
-      <c r="D21">
-        <v>82947.08064</v>
-      </c>
-      <c r="E21">
-        <v>303.14</v>
-      </c>
-      <c r="F21">
-        <v>295.5</v>
-      </c>
-      <c r="G21">
-        <v>101562.923784</v>
-      </c>
-      <c r="H21">
-        <v>237527.5263024</v>
-      </c>
-      <c r="I21">
-        <v>128176.6847232</v>
-      </c>
-      <c r="J21">
-        <v>252971.78135520002</v>
-      </c>
-      <c r="K21">
-        <v>74673.37257600001</v>
-      </c>
-      <c r="L21">
-        <v>152032.5429744</v>
-      </c>
-      <c r="M21">
-        <v>116317.7031648</v>
-      </c>
-      <c r="N21">
-        <v>245732.2867992</v>
-      </c>
-      <c r="O21">
-        <v>1.8532679853150253</v>
-      </c>
-      <c r="P21">
-        <v>1.9557777009714101</v>
-      </c>
-      <c r="Q21">
-        <v>1.1795040422691863</v>
-      </c>
-      <c r="R21">
-        <v>1.9121506532311674</v>
-      </c>
-      <c r="S21">
-        <v>690.0700381786789</v>
-      </c>
-      <c r="T21">
-        <v>44.99680413605927</v>
+        <v>38.802499891034415</v>
       </c>
     </row>
   </sheetData>

</xml_diff>